<commit_message>
update data: remove redundant column
</commit_message>
<xml_diff>
--- a/data/common-value-auction.xlsx
+++ b/data/common-value-auction.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,30 +375,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Treatment</t>
+          <t>Round</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Round</t>
+          <t>ID_self</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ID_self</t>
+          <t>ID_partner</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>ID_partner</t>
+          <t>Signal</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Signal</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Bid</t>
         </is>
@@ -416,24 +411,19 @@
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>8.970000000000001</v>
       </c>
       <c r="H2">
-        <v>8.970000000000001</v>
-      </c>
-      <c r="I2">
         <v>4</v>
       </c>
     </row>
@@ -449,24 +439,19 @@
       <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>6.27</v>
       </c>
       <c r="H3">
-        <v>6.27</v>
-      </c>
-      <c r="I3">
         <v>3</v>
       </c>
     </row>
@@ -482,24 +467,19 @@
       <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>2.06</v>
       </c>
       <c r="H4">
-        <v>2.06</v>
-      </c>
-      <c r="I4">
         <v>2</v>
       </c>
     </row>
@@ -515,24 +495,19 @@
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>0.39</v>
       </c>
       <c r="H5">
-        <v>0.39</v>
-      </c>
-      <c r="I5">
         <v>0.6</v>
       </c>
     </row>
@@ -548,24 +523,19 @@
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G6">
-        <v>9</v>
+        <v>3.15</v>
       </c>
       <c r="H6">
-        <v>3.15</v>
-      </c>
-      <c r="I6">
         <v>1.02</v>
       </c>
     </row>
@@ -581,24 +551,19 @@
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G7">
-        <v>8</v>
+        <v>0.58</v>
       </c>
       <c r="H7">
-        <v>0.58</v>
-      </c>
-      <c r="I7">
         <v>1</v>
       </c>
     </row>
@@ -614,24 +579,19 @@
       <c r="C8">
         <v>10</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>2.24</v>
       </c>
       <c r="H8">
-        <v>2.24</v>
-      </c>
-      <c r="I8">
         <v>2</v>
       </c>
     </row>
@@ -647,24 +607,19 @@
       <c r="C9">
         <v>10</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G9">
-        <v>6</v>
+        <v>5.78</v>
       </c>
       <c r="H9">
-        <v>5.78</v>
-      </c>
-      <c r="I9">
         <v>3</v>
       </c>
     </row>
@@ -680,24 +635,19 @@
       <c r="C10">
         <v>10</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>1.91</v>
       </c>
       <c r="H10">
-        <v>1.91</v>
-      </c>
-      <c r="I10">
         <v>1.03</v>
       </c>
     </row>
@@ -713,24 +663,19 @@
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>1.73</v>
       </c>
       <c r="H11">
-        <v>1.73</v>
-      </c>
-      <c r="I11">
         <v>3</v>
       </c>
     </row>
@@ -746,24 +691,19 @@
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>8.75</v>
       </c>
       <c r="H12">
-        <v>8.75</v>
-      </c>
-      <c r="I12">
         <v>6</v>
       </c>
     </row>
@@ -779,24 +719,19 @@
       <c r="C13">
         <v>10</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>3.98</v>
       </c>
       <c r="H13">
-        <v>3.98</v>
-      </c>
-      <c r="I13">
         <v>5</v>
       </c>
     </row>
@@ -812,24 +747,19 @@
       <c r="C14">
         <v>10</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G14">
-        <v>6</v>
+        <v>4.58</v>
       </c>
       <c r="H14">
-        <v>4.58</v>
-      </c>
-      <c r="I14">
         <v>3.08</v>
       </c>
     </row>
@@ -845,24 +775,19 @@
       <c r="C15">
         <v>10</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <v>8</v>
+        <v>3.51</v>
       </c>
       <c r="H15">
-        <v>3.51</v>
-      </c>
-      <c r="I15">
         <v>3.6</v>
       </c>
     </row>
@@ -878,24 +803,19 @@
       <c r="C16">
         <v>10</v>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>10</v>
+        <v>5.35</v>
       </c>
       <c r="H16">
-        <v>5.35</v>
-      </c>
-      <c r="I16">
         <v>2.5</v>
       </c>
     </row>
@@ -911,24 +831,19 @@
       <c r="C17">
         <v>10</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D17">
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G17">
-        <v>3</v>
+        <v>3.36</v>
       </c>
       <c r="H17">
-        <v>3.36</v>
-      </c>
-      <c r="I17">
         <v>5</v>
       </c>
     </row>
@@ -944,24 +859,19 @@
       <c r="C18">
         <v>10</v>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G18">
-        <v>9</v>
+        <v>0.21</v>
       </c>
       <c r="H18">
-        <v>0.21</v>
-      </c>
-      <c r="I18">
         <v>5</v>
       </c>
     </row>
@@ -977,24 +887,19 @@
       <c r="C19">
         <v>10</v>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D19">
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>5.6</v>
       </c>
       <c r="H19">
-        <v>5.6</v>
-      </c>
-      <c r="I19">
         <v>3</v>
       </c>
     </row>
@@ -1010,24 +915,19 @@
       <c r="C20">
         <v>10</v>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D20">
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G20">
-        <v>7</v>
+        <v>4.82</v>
       </c>
       <c r="H20">
-        <v>4.82</v>
-      </c>
-      <c r="I20">
         <v>4.26</v>
       </c>
     </row>
@@ -1043,24 +943,19 @@
       <c r="C21">
         <v>10</v>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D21">
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G21">
-        <v>5</v>
+        <v>6.22</v>
       </c>
       <c r="H21">
-        <v>6.22</v>
-      </c>
-      <c r="I21">
         <v>7.22</v>
       </c>
     </row>
@@ -1076,24 +971,19 @@
       <c r="C22">
         <v>5</v>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D22">
+        <v>1</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G22">
-        <v>10</v>
+        <v>0.91</v>
       </c>
       <c r="H22">
-        <v>0.91</v>
-      </c>
-      <c r="I22">
         <v>1</v>
       </c>
     </row>
@@ -1109,24 +999,19 @@
       <c r="C23">
         <v>5</v>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D23">
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G23">
-        <v>7</v>
+        <v>0.76</v>
       </c>
       <c r="H23">
-        <v>0.76</v>
-      </c>
-      <c r="I23">
         <v>1</v>
       </c>
     </row>
@@ -1142,24 +1027,19 @@
       <c r="C24">
         <v>5</v>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G24">
-        <v>6</v>
+        <v>3.43</v>
       </c>
       <c r="H24">
-        <v>3.43</v>
-      </c>
-      <c r="I24">
         <v>2.51</v>
       </c>
     </row>
@@ -1175,24 +1055,19 @@
       <c r="C25">
         <v>5</v>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G25">
-        <v>9</v>
+        <v>4.16</v>
       </c>
       <c r="H25">
-        <v>4.16</v>
-      </c>
-      <c r="I25">
         <v>3.91</v>
       </c>
     </row>
@@ -1208,24 +1083,19 @@
       <c r="C26">
         <v>5</v>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F26">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G26">
-        <v>8</v>
+        <v>2.04</v>
       </c>
       <c r="H26">
-        <v>2.04</v>
-      </c>
-      <c r="I26">
         <v>1.5</v>
       </c>
     </row>
@@ -1241,24 +1111,19 @@
       <c r="C27">
         <v>5</v>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F27">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G27">
-        <v>3</v>
+        <v>4.66</v>
       </c>
       <c r="H27">
-        <v>4.66</v>
-      </c>
-      <c r="I27">
         <v>1.01</v>
       </c>
     </row>
@@ -1274,24 +1139,19 @@
       <c r="C28">
         <v>5</v>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D28">
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F28">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>0.63</v>
       </c>
       <c r="H28">
-        <v>0.63</v>
-      </c>
-      <c r="I28">
         <v>1.51</v>
       </c>
     </row>
@@ -1307,24 +1167,19 @@
       <c r="C29">
         <v>5</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D29">
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F29">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G29">
-        <v>5</v>
+        <v>2.84</v>
       </c>
       <c r="H29">
-        <v>2.84</v>
-      </c>
-      <c r="I29">
         <v>1.45</v>
       </c>
     </row>
@@ -1340,24 +1195,19 @@
       <c r="C30">
         <v>5</v>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D30">
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F30">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G30">
-        <v>4</v>
+        <v>3.96</v>
       </c>
       <c r="H30">
-        <v>3.96</v>
-      </c>
-      <c r="I30">
         <v>2</v>
       </c>
     </row>
@@ -1373,24 +1223,19 @@
       <c r="C31">
         <v>5</v>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D31">
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="H31">
-        <v>0.68</v>
-      </c>
-      <c r="I31">
         <v>2.56</v>
       </c>
     </row>
@@ -1406,24 +1251,19 @@
       <c r="C32">
         <v>10</v>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D32">
+        <v>1</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G32">
-        <v>6</v>
+        <v>1.97</v>
       </c>
       <c r="H32">
-        <v>1.97</v>
-      </c>
-      <c r="I32">
         <v>3</v>
       </c>
     </row>
@@ -1439,24 +1279,19 @@
       <c r="C33">
         <v>10</v>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D33">
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G33">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="H33">
-        <v>2.7</v>
-      </c>
-      <c r="I33">
         <v>3</v>
       </c>
     </row>
@@ -1472,24 +1307,19 @@
       <c r="C34">
         <v>10</v>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D34">
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>5.61</v>
       </c>
       <c r="H34">
-        <v>5.61</v>
-      </c>
-      <c r="I34">
         <v>4</v>
       </c>
     </row>
@@ -1505,24 +1335,19 @@
       <c r="C35">
         <v>10</v>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D35">
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G35">
-        <v>5</v>
+        <v>6.72</v>
       </c>
       <c r="H35">
-        <v>6.72</v>
-      </c>
-      <c r="I35">
         <v>5</v>
       </c>
     </row>
@@ -1538,26 +1363,21 @@
       <c r="C36">
         <v>10</v>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D36">
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G36">
-        <v>4</v>
+        <v>0.57</v>
       </c>
       <c r="H36">
         <v>0.57</v>
       </c>
-      <c r="I36">
-        <v>0.57</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -1571,24 +1391,19 @@
       <c r="C37">
         <v>10</v>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D37">
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F37">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>5.87</v>
       </c>
       <c r="H37">
-        <v>5.87</v>
-      </c>
-      <c r="I37">
         <v>2</v>
       </c>
     </row>
@@ -1604,24 +1419,19 @@
       <c r="C38">
         <v>10</v>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D38">
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F38">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G38">
-        <v>8</v>
+        <v>0.03</v>
       </c>
       <c r="H38">
-        <v>0.03</v>
-      </c>
-      <c r="I38">
         <v>4</v>
       </c>
     </row>
@@ -1637,24 +1447,19 @@
       <c r="C39">
         <v>10</v>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D39">
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G39">
-        <v>7</v>
+        <v>1.18</v>
       </c>
       <c r="H39">
-        <v>1.18</v>
-      </c>
-      <c r="I39">
         <v>2.57</v>
       </c>
     </row>
@@ -1670,24 +1475,19 @@
       <c r="C40">
         <v>5</v>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D40">
+        <v>1</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G40">
-        <v>6</v>
+        <v>1.79</v>
       </c>
       <c r="H40">
-        <v>1.79</v>
-      </c>
-      <c r="I40">
         <v>1.5</v>
       </c>
     </row>
@@ -1703,24 +1503,19 @@
       <c r="C41">
         <v>5</v>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D41">
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G41">
-        <v>4</v>
+        <v>1.41</v>
       </c>
       <c r="H41">
-        <v>1.41</v>
-      </c>
-      <c r="I41">
         <v>2</v>
       </c>
     </row>
@@ -1736,26 +1531,21 @@
       <c r="C42">
         <v>5</v>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D42">
+        <v>1</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G42">
-        <v>8</v>
+        <v>0.09</v>
       </c>
       <c r="H42">
         <v>0.09</v>
       </c>
-      <c r="I42">
-        <v>0.09</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -1769,24 +1559,19 @@
       <c r="C43">
         <v>5</v>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D43">
+        <v>1</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>3.47</v>
       </c>
       <c r="H43">
-        <v>3.47</v>
-      </c>
-      <c r="I43">
         <v>2.01</v>
       </c>
     </row>
@@ -1802,24 +1587,19 @@
       <c r="C44">
         <v>5</v>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D44">
+        <v>1</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G44">
-        <v>7</v>
+        <v>4.09</v>
       </c>
       <c r="H44">
-        <v>4.09</v>
-      </c>
-      <c r="I44">
         <v>1.5</v>
       </c>
     </row>
@@ -1835,24 +1615,19 @@
       <c r="C45">
         <v>5</v>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D45">
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F45">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>4.96</v>
       </c>
       <c r="H45">
-        <v>4.96</v>
-      </c>
-      <c r="I45">
         <v>2.75</v>
       </c>
     </row>
@@ -1868,24 +1643,19 @@
       <c r="C46">
         <v>5</v>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D46">
+        <v>1</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G46">
-        <v>5</v>
+        <v>0.38</v>
       </c>
       <c r="H46">
-        <v>0.38</v>
-      </c>
-      <c r="I46">
         <v>0.5</v>
       </c>
     </row>
@@ -1901,24 +1671,19 @@
       <c r="C47">
         <v>5</v>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D47">
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F47">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G47">
-        <v>3</v>
+        <v>1.69</v>
       </c>
       <c r="H47">
-        <v>1.69</v>
-      </c>
-      <c r="I47">
         <v>2.01</v>
       </c>
     </row>
@@ -1934,24 +1699,19 @@
       <c r="C48">
         <v>10</v>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D48">
+        <v>1</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G48">
-        <v>8</v>
+        <v>1.55</v>
       </c>
       <c r="H48">
-        <v>1.55</v>
-      </c>
-      <c r="I48">
         <v>3.55</v>
       </c>
     </row>
@@ -1967,24 +1727,19 @@
       <c r="C49">
         <v>10</v>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D49">
+        <v>1</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G49">
-        <v>7</v>
+        <v>8.66</v>
       </c>
       <c r="H49">
-        <v>8.66</v>
-      </c>
-      <c r="I49">
         <v>8</v>
       </c>
     </row>
@@ -2000,24 +1755,19 @@
       <c r="C50">
         <v>10</v>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D50">
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G50">
-        <v>10</v>
+        <v>7.85</v>
       </c>
       <c r="H50">
-        <v>7.85</v>
-      </c>
-      <c r="I50">
         <v>3.5</v>
       </c>
     </row>
@@ -2033,24 +1783,19 @@
       <c r="C51">
         <v>10</v>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D51">
+        <v>1</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G51">
-        <v>5</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H51">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="I51">
         <v>8</v>
       </c>
     </row>
@@ -2066,24 +1811,19 @@
       <c r="C52">
         <v>10</v>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D52">
+        <v>1</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F52">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G52">
-        <v>4</v>
+        <v>9.1</v>
       </c>
       <c r="H52">
-        <v>9.1</v>
-      </c>
-      <c r="I52">
         <v>4</v>
       </c>
     </row>
@@ -2099,24 +1839,19 @@
       <c r="C53">
         <v>10</v>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D53">
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F53">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G53">
-        <v>9</v>
+        <v>2.12</v>
       </c>
       <c r="H53">
-        <v>2.12</v>
-      </c>
-      <c r="I53">
         <v>3</v>
       </c>
     </row>
@@ -2132,24 +1867,19 @@
       <c r="C54">
         <v>10</v>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D54">
+        <v>1</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F54">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G54">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="H54">
-        <v>5.5</v>
-      </c>
-      <c r="I54">
         <v>4</v>
       </c>
     </row>
@@ -2165,24 +1895,19 @@
       <c r="C55">
         <v>10</v>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D55">
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F55">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>4.25</v>
       </c>
       <c r="H55">
-        <v>4.25</v>
-      </c>
-      <c r="I55">
         <v>2</v>
       </c>
     </row>
@@ -2198,24 +1923,19 @@
       <c r="C56">
         <v>10</v>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D56">
+        <v>1</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F56">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G56">
-        <v>6</v>
+        <v>1.87</v>
       </c>
       <c r="H56">
-        <v>1.87</v>
-      </c>
-      <c r="I56">
         <v>1</v>
       </c>
     </row>
@@ -2231,24 +1951,19 @@
       <c r="C57">
         <v>10</v>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D57">
+        <v>1</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G57">
-        <v>3</v>
+        <v>7.01</v>
       </c>
       <c r="H57">
-        <v>7.01</v>
-      </c>
-      <c r="I57">
         <v>5</v>
       </c>
     </row>
@@ -2264,24 +1979,19 @@
       <c r="C58">
         <v>5</v>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D58">
+        <v>1</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G58">
-        <v>6</v>
+        <v>2.41</v>
       </c>
       <c r="H58">
-        <v>2.41</v>
-      </c>
-      <c r="I58">
         <v>1.51</v>
       </c>
     </row>
@@ -2297,24 +2007,19 @@
       <c r="C59">
         <v>5</v>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D59">
+        <v>1</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F59">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G59">
-        <v>7</v>
+        <v>1.82</v>
       </c>
       <c r="H59">
-        <v>1.82</v>
-      </c>
-      <c r="I59">
         <v>2</v>
       </c>
     </row>
@@ -2330,24 +2035,19 @@
       <c r="C60">
         <v>5</v>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D60">
+        <v>1</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F60">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G60">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H60">
-        <v>3</v>
-      </c>
-      <c r="I60">
         <v>1.15</v>
       </c>
     </row>
@@ -2363,24 +2063,19 @@
       <c r="C61">
         <v>5</v>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D61">
+        <v>1</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F61">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G61">
-        <v>8</v>
+        <v>2.87</v>
       </c>
       <c r="H61">
-        <v>2.87</v>
-      </c>
-      <c r="I61">
         <v>2</v>
       </c>
     </row>
@@ -2396,24 +2091,19 @@
       <c r="C62">
         <v>5</v>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D62">
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F62">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G62">
-        <v>9</v>
+        <v>4.86</v>
       </c>
       <c r="H62">
-        <v>4.86</v>
-      </c>
-      <c r="I62">
         <v>1.5</v>
       </c>
     </row>
@@ -2429,24 +2119,19 @@
       <c r="C63">
         <v>5</v>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D63">
+        <v>1</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F63">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G63">
-        <v>1</v>
+        <v>0.23</v>
       </c>
       <c r="H63">
-        <v>0.23</v>
-      </c>
-      <c r="I63">
         <v>0.5</v>
       </c>
     </row>
@@ -2462,24 +2147,19 @@
       <c r="C64">
         <v>5</v>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D64">
+        <v>1</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F64">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G64">
-        <v>2</v>
+        <v>3.67</v>
       </c>
       <c r="H64">
-        <v>3.67</v>
-      </c>
-      <c r="I64">
         <v>2.25</v>
       </c>
     </row>
@@ -2495,24 +2175,19 @@
       <c r="C65">
         <v>5</v>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D65">
+        <v>1</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F65">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G65">
-        <v>4</v>
+        <v>1.84</v>
       </c>
       <c r="H65">
-        <v>1.84</v>
-      </c>
-      <c r="I65">
         <v>2.01</v>
       </c>
     </row>
@@ -2528,24 +2203,19 @@
       <c r="C66">
         <v>5</v>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D66">
+        <v>1</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F66">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G66">
-        <v>5</v>
+        <v>2.12</v>
       </c>
       <c r="H66">
-        <v>2.12</v>
-      </c>
-      <c r="I66">
         <v>1</v>
       </c>
     </row>
@@ -2561,24 +2231,19 @@
       <c r="C67">
         <v>5</v>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D67">
+        <v>1</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G67">
-        <v>3</v>
+        <v>0.37</v>
       </c>
       <c r="H67">
-        <v>0.37</v>
-      </c>
-      <c r="I67">
         <v>1.5</v>
       </c>
     </row>
@@ -2594,24 +2259,19 @@
       <c r="C68">
         <v>10</v>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D68">
+        <v>1</v>
       </c>
       <c r="E68">
         <v>1</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G68">
-        <v>7</v>
+        <v>2.98</v>
       </c>
       <c r="H68">
-        <v>2.98</v>
-      </c>
-      <c r="I68">
         <v>2.97</v>
       </c>
     </row>
@@ -2627,24 +2287,19 @@
       <c r="C69">
         <v>10</v>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D69">
+        <v>1</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F69">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G69">
-        <v>8</v>
+        <v>0.45</v>
       </c>
       <c r="H69">
-        <v>0.45</v>
-      </c>
-      <c r="I69">
         <v>1.5</v>
       </c>
     </row>
@@ -2660,24 +2315,19 @@
       <c r="C70">
         <v>10</v>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D70">
+        <v>1</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F70">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G70">
-        <v>4</v>
+        <v>9.92</v>
       </c>
       <c r="H70">
-        <v>9.92</v>
-      </c>
-      <c r="I70">
         <v>5</v>
       </c>
     </row>
@@ -2693,24 +2343,19 @@
       <c r="C71">
         <v>10</v>
       </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D71">
+        <v>1</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G71">
-        <v>3</v>
+        <v>6.76</v>
       </c>
       <c r="H71">
-        <v>6.76</v>
-      </c>
-      <c r="I71">
         <v>5</v>
       </c>
     </row>
@@ -2726,24 +2371,19 @@
       <c r="C72">
         <v>10</v>
       </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D72">
+        <v>1</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F72">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G72">
-        <v>10</v>
+        <v>0.63</v>
       </c>
       <c r="H72">
-        <v>0.63</v>
-      </c>
-      <c r="I72">
         <v>0.75</v>
       </c>
     </row>
@@ -2759,24 +2399,19 @@
       <c r="C73">
         <v>10</v>
       </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D73">
+        <v>1</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F73">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G73">
-        <v>9</v>
+        <v>1.31</v>
       </c>
       <c r="H73">
-        <v>1.31</v>
-      </c>
-      <c r="I73">
         <v>3</v>
       </c>
     </row>
@@ -2792,24 +2427,19 @@
       <c r="C74">
         <v>10</v>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D74">
+        <v>1</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F74">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>5.73</v>
       </c>
       <c r="H74">
-        <v>5.73</v>
-      </c>
-      <c r="I74">
         <v>5.5</v>
       </c>
     </row>
@@ -2825,24 +2455,19 @@
       <c r="C75">
         <v>10</v>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D75">
+        <v>1</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F75">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G75">
-        <v>2</v>
+        <v>7.42</v>
       </c>
       <c r="H75">
-        <v>7.42</v>
-      </c>
-      <c r="I75">
         <v>4.02</v>
       </c>
     </row>
@@ -2858,24 +2483,19 @@
       <c r="C76">
         <v>10</v>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D76">
+        <v>1</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F76">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G76">
-        <v>6</v>
+        <v>3.78</v>
       </c>
       <c r="H76">
-        <v>3.78</v>
-      </c>
-      <c r="I76">
         <v>4</v>
       </c>
     </row>
@@ -2891,24 +2511,19 @@
       <c r="C77">
         <v>10</v>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D77">
+        <v>1</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G77">
-        <v>5</v>
+        <v>6.33</v>
       </c>
       <c r="H77">
-        <v>6.33</v>
-      </c>
-      <c r="I77">
         <v>5</v>
       </c>
     </row>
@@ -2924,24 +2539,19 @@
       <c r="C78">
         <v>5</v>
       </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D78">
+        <v>1</v>
       </c>
       <c r="E78">
         <v>1</v>
       </c>
       <c r="F78">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G78">
-        <v>7</v>
+        <v>3.06</v>
       </c>
       <c r="H78">
-        <v>3.06</v>
-      </c>
-      <c r="I78">
         <v>2.5</v>
       </c>
     </row>
@@ -2957,24 +2567,19 @@
       <c r="C79">
         <v>5</v>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D79">
+        <v>1</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F79">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G79">
-        <v>9</v>
+        <v>4.63</v>
       </c>
       <c r="H79">
-        <v>4.63</v>
-      </c>
-      <c r="I79">
         <v>2.53</v>
       </c>
     </row>
@@ -2990,24 +2595,19 @@
       <c r="C80">
         <v>5</v>
       </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D80">
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F80">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G80">
-        <v>10</v>
+        <v>3.52</v>
       </c>
       <c r="H80">
-        <v>3.52</v>
-      </c>
-      <c r="I80">
         <v>3.53</v>
       </c>
     </row>
@@ -3023,24 +2623,19 @@
       <c r="C81">
         <v>5</v>
       </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D81">
+        <v>1</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F81">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G81">
-        <v>8</v>
+        <v>4.84</v>
       </c>
       <c r="H81">
-        <v>4.84</v>
-      </c>
-      <c r="I81">
         <v>2.5</v>
       </c>
     </row>
@@ -3056,24 +2651,19 @@
       <c r="C82">
         <v>5</v>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D82">
+        <v>1</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F82">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G82">
-        <v>6</v>
+        <v>4.53</v>
       </c>
       <c r="H82">
-        <v>4.53</v>
-      </c>
-      <c r="I82">
         <v>2.71</v>
       </c>
     </row>
@@ -3089,24 +2679,19 @@
       <c r="C83">
         <v>5</v>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D83">
+        <v>1</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G83">
-        <v>5</v>
+        <v>1.96</v>
       </c>
       <c r="H83">
-        <v>1.96</v>
-      </c>
-      <c r="I83">
         <v>2.5</v>
       </c>
     </row>
@@ -3122,24 +2707,19 @@
       <c r="C84">
         <v>5</v>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D84">
+        <v>1</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F84">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>1.56</v>
       </c>
       <c r="H84">
-        <v>1.56</v>
-      </c>
-      <c r="I84">
         <v>2.65</v>
       </c>
     </row>
@@ -3155,24 +2735,19 @@
       <c r="C85">
         <v>5</v>
       </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D85">
+        <v>1</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F85">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G85">
-        <v>4</v>
+        <v>0.87</v>
       </c>
       <c r="H85">
-        <v>0.87</v>
-      </c>
-      <c r="I85">
         <v>1.57</v>
       </c>
     </row>
@@ -3188,24 +2763,19 @@
       <c r="C86">
         <v>5</v>
       </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D86">
+        <v>1</v>
       </c>
       <c r="E86">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F86">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G86">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="H86">
-        <v>3.2</v>
-      </c>
-      <c r="I86">
         <v>1.99</v>
       </c>
     </row>
@@ -3221,24 +2791,19 @@
       <c r="C87">
         <v>5</v>
       </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D87">
+        <v>1</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F87">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G87">
-        <v>3</v>
+        <v>4.91</v>
       </c>
       <c r="H87">
-        <v>4.91</v>
-      </c>
-      <c r="I87">
         <v>2.52</v>
       </c>
     </row>
@@ -3254,24 +2819,19 @@
       <c r="C88">
         <v>10</v>
       </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D88">
+        <v>1</v>
       </c>
       <c r="E88">
         <v>1</v>
       </c>
       <c r="F88">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G88">
-        <v>3</v>
+        <v>0.33</v>
       </c>
       <c r="H88">
-        <v>0.33</v>
-      </c>
-      <c r="I88">
         <v>0.8</v>
       </c>
     </row>
@@ -3287,24 +2847,19 @@
       <c r="C89">
         <v>10</v>
       </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D89">
+        <v>1</v>
       </c>
       <c r="E89">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F89">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G89">
-        <v>10</v>
+        <v>5.47</v>
       </c>
       <c r="H89">
-        <v>5.47</v>
-      </c>
-      <c r="I89">
         <v>5.01</v>
       </c>
     </row>
@@ -3320,24 +2875,19 @@
       <c r="C90">
         <v>10</v>
       </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D90">
+        <v>1</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F90">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>4.09</v>
       </c>
       <c r="H90">
-        <v>4.09</v>
-      </c>
-      <c r="I90">
         <v>4</v>
       </c>
     </row>
@@ -3353,24 +2903,19 @@
       <c r="C91">
         <v>10</v>
       </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D91">
+        <v>1</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F91">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G91">
-        <v>7</v>
+        <v>7.12</v>
       </c>
       <c r="H91">
-        <v>7.12</v>
-      </c>
-      <c r="I91">
         <v>4</v>
       </c>
     </row>
@@ -3386,24 +2931,19 @@
       <c r="C92">
         <v>10</v>
       </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D92">
+        <v>1</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F92">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G92">
-        <v>9</v>
+        <v>1.27</v>
       </c>
       <c r="H92">
-        <v>1.27</v>
-      </c>
-      <c r="I92">
         <v>3</v>
       </c>
     </row>
@@ -3419,24 +2959,19 @@
       <c r="C93">
         <v>10</v>
       </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D93">
+        <v>1</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F93">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G93">
-        <v>8</v>
+        <v>6.28</v>
       </c>
       <c r="H93">
-        <v>6.28</v>
-      </c>
-      <c r="I93">
         <v>4</v>
       </c>
     </row>
@@ -3452,24 +2987,19 @@
       <c r="C94">
         <v>10</v>
       </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D94">
+        <v>1</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G94">
-        <v>4</v>
+        <v>1.01</v>
       </c>
       <c r="H94">
-        <v>1.01</v>
-      </c>
-      <c r="I94">
         <v>2.2</v>
       </c>
     </row>
@@ -3485,24 +3015,19 @@
       <c r="C95">
         <v>10</v>
       </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D95">
+        <v>1</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F95">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G95">
-        <v>6</v>
+        <v>6.04</v>
       </c>
       <c r="H95">
-        <v>6.04</v>
-      </c>
-      <c r="I95">
         <v>4.88</v>
       </c>
     </row>
@@ -3518,24 +3043,19 @@
       <c r="C96">
         <v>10</v>
       </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D96">
+        <v>1</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F96">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G96">
-        <v>5</v>
+        <v>7.14</v>
       </c>
       <c r="H96">
-        <v>7.14</v>
-      </c>
-      <c r="I96">
         <v>3.68</v>
       </c>
     </row>
@@ -3551,24 +3071,19 @@
       <c r="C97">
         <v>10</v>
       </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D97">
+        <v>1</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G97">
-        <v>2</v>
+        <v>5.74</v>
       </c>
       <c r="H97">
-        <v>5.74</v>
-      </c>
-      <c r="I97">
         <v>5</v>
       </c>
     </row>
@@ -3584,24 +3099,19 @@
       <c r="C98">
         <v>5</v>
       </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D98">
+        <v>1</v>
       </c>
       <c r="E98">
         <v>1</v>
       </c>
       <c r="F98">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G98">
-        <v>3</v>
+        <v>0.89</v>
       </c>
       <c r="H98">
-        <v>0.89</v>
-      </c>
-      <c r="I98">
         <v>0.45</v>
       </c>
     </row>
@@ -3617,24 +3127,19 @@
       <c r="C99">
         <v>5</v>
       </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D99">
+        <v>1</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F99">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G99">
-        <v>10</v>
+        <v>3.55</v>
       </c>
       <c r="H99">
-        <v>3.55</v>
-      </c>
-      <c r="I99">
         <v>2.99</v>
       </c>
     </row>
@@ -3650,24 +3155,19 @@
       <c r="C100">
         <v>5</v>
       </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D100">
+        <v>1</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F100">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G100">
-        <v>1</v>
+        <v>4.53</v>
       </c>
       <c r="H100">
-        <v>4.53</v>
-      </c>
-      <c r="I100">
         <v>3.55</v>
       </c>
     </row>
@@ -3683,24 +3183,19 @@
       <c r="C101">
         <v>5</v>
       </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D101">
+        <v>1</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F101">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G101">
-        <v>8</v>
+        <v>3.29</v>
       </c>
       <c r="H101">
-        <v>3.29</v>
-      </c>
-      <c r="I101">
         <v>3</v>
       </c>
     </row>
@@ -3716,24 +3211,19 @@
       <c r="C102">
         <v>5</v>
       </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D102">
+        <v>1</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F102">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G102">
-        <v>6</v>
+        <v>3.13</v>
       </c>
       <c r="H102">
-        <v>3.13</v>
-      </c>
-      <c r="I102">
         <v>2.01</v>
       </c>
     </row>
@@ -3749,24 +3239,19 @@
       <c r="C103">
         <v>5</v>
       </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D103">
+        <v>1</v>
       </c>
       <c r="E103">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F103">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G103">
-        <v>5</v>
+        <v>2.79</v>
       </c>
       <c r="H103">
-        <v>2.79</v>
-      </c>
-      <c r="I103">
         <v>3</v>
       </c>
     </row>
@@ -3782,24 +3267,19 @@
       <c r="C104">
         <v>5</v>
       </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D104">
+        <v>1</v>
       </c>
       <c r="E104">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F104">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G104">
-        <v>9</v>
+        <v>2.78</v>
       </c>
       <c r="H104">
-        <v>2.78</v>
-      </c>
-      <c r="I104">
         <v>1.05</v>
       </c>
     </row>
@@ -3815,24 +3295,19 @@
       <c r="C105">
         <v>5</v>
       </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D105">
+        <v>1</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F105">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G105">
-        <v>4</v>
+        <v>2.28</v>
       </c>
       <c r="H105">
-        <v>2.28</v>
-      </c>
-      <c r="I105">
         <v>2.01</v>
       </c>
     </row>
@@ -3848,24 +3323,19 @@
       <c r="C106">
         <v>5</v>
       </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D106">
+        <v>1</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F106">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G106">
-        <v>7</v>
+        <v>4.8</v>
       </c>
       <c r="H106">
-        <v>4.8</v>
-      </c>
-      <c r="I106">
         <v>2.41</v>
       </c>
     </row>
@@ -3881,24 +3351,19 @@
       <c r="C107">
         <v>5</v>
       </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D107">
+        <v>1</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F107">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G107">
-        <v>2</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H107">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="I107">
         <v>1.5</v>
       </c>
     </row>
@@ -3914,24 +3379,19 @@
       <c r="C108">
         <v>10</v>
       </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D108">
+        <v>1</v>
       </c>
       <c r="E108">
         <v>1</v>
       </c>
       <c r="F108">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G108">
-        <v>7</v>
+        <v>5.24</v>
       </c>
       <c r="H108">
-        <v>5.24</v>
-      </c>
-      <c r="I108">
         <v>3</v>
       </c>
     </row>
@@ -3947,24 +3407,19 @@
       <c r="C109">
         <v>10</v>
       </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D109">
+        <v>1</v>
       </c>
       <c r="E109">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F109">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G109">
-        <v>8</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="H109">
-        <v>8.529999999999999</v>
-      </c>
-      <c r="I109">
         <v>4.5</v>
       </c>
     </row>
@@ -3980,24 +3435,19 @@
       <c r="C110">
         <v>10</v>
       </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D110">
+        <v>1</v>
       </c>
       <c r="E110">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F110">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G110">
-        <v>10</v>
+        <v>5.48</v>
       </c>
       <c r="H110">
-        <v>5.48</v>
-      </c>
-      <c r="I110">
         <v>5.02</v>
       </c>
     </row>
@@ -4013,24 +3463,19 @@
       <c r="C111">
         <v>10</v>
       </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D111">
+        <v>1</v>
       </c>
       <c r="E111">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F111">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G111">
-        <v>9</v>
+        <v>7.94</v>
       </c>
       <c r="H111">
-        <v>7.94</v>
-      </c>
-      <c r="I111">
         <v>8</v>
       </c>
     </row>
@@ -4046,24 +3491,19 @@
       <c r="C112">
         <v>10</v>
       </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D112">
+        <v>1</v>
       </c>
       <c r="E112">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F112">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G112">
-        <v>6</v>
+        <v>3.64</v>
       </c>
       <c r="H112">
-        <v>3.64</v>
-      </c>
-      <c r="I112">
         <v>0.5</v>
       </c>
     </row>
@@ -4079,24 +3519,19 @@
       <c r="C113">
         <v>10</v>
       </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D113">
+        <v>1</v>
       </c>
       <c r="E113">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F113">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G113">
-        <v>5</v>
+        <v>3.25</v>
       </c>
       <c r="H113">
-        <v>3.25</v>
-      </c>
-      <c r="I113">
         <v>2</v>
       </c>
     </row>
@@ -4112,24 +3547,19 @@
       <c r="C114">
         <v>10</v>
       </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D114">
+        <v>1</v>
       </c>
       <c r="E114">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F114">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G114">
-        <v>1</v>
+        <v>1.62</v>
       </c>
       <c r="H114">
-        <v>1.62</v>
-      </c>
-      <c r="I114">
         <v>3.5</v>
       </c>
     </row>
@@ -4145,24 +3575,19 @@
       <c r="C115">
         <v>10</v>
       </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D115">
+        <v>1</v>
       </c>
       <c r="E115">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F115">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G115">
-        <v>2</v>
+        <v>2.62</v>
       </c>
       <c r="H115">
-        <v>2.62</v>
-      </c>
-      <c r="I115">
         <v>4</v>
       </c>
     </row>
@@ -4178,24 +3603,19 @@
       <c r="C116">
         <v>10</v>
       </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D116">
+        <v>1</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F116">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G116">
-        <v>4</v>
+        <v>2.07</v>
       </c>
       <c r="H116">
-        <v>2.07</v>
-      </c>
-      <c r="I116">
         <v>2</v>
       </c>
     </row>
@@ -4211,24 +3631,19 @@
       <c r="C117">
         <v>10</v>
       </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D117">
+        <v>1</v>
       </c>
       <c r="E117">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F117">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G117">
-        <v>3</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="H117">
-        <v>9.050000000000001</v>
-      </c>
-      <c r="I117">
         <v>4.5</v>
       </c>
     </row>
@@ -4244,24 +3659,19 @@
       <c r="C118">
         <v>5</v>
       </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D118">
+        <v>1</v>
       </c>
       <c r="E118">
         <v>1</v>
       </c>
       <c r="F118">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G118">
-        <v>10</v>
+        <v>5.48</v>
       </c>
       <c r="H118">
-        <v>5.48</v>
-      </c>
-      <c r="I118">
         <v>5.02</v>
       </c>
     </row>
@@ -4277,24 +3687,19 @@
       <c r="C119">
         <v>5</v>
       </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D119">
+        <v>1</v>
       </c>
       <c r="E119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F119">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G119">
-        <v>7</v>
+        <v>5.24</v>
       </c>
       <c r="H119">
-        <v>5.24</v>
-      </c>
-      <c r="I119">
         <v>3</v>
       </c>
     </row>
@@ -4310,24 +3715,19 @@
       <c r="C120">
         <v>5</v>
       </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D120">
+        <v>1</v>
       </c>
       <c r="E120">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F120">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G120">
-        <v>8</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="H120">
-        <v>8.529999999999999</v>
-      </c>
-      <c r="I120">
         <v>4.5</v>
       </c>
     </row>
@@ -4343,24 +3743,19 @@
       <c r="C121">
         <v>5</v>
       </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D121">
+        <v>1</v>
       </c>
       <c r="E121">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F121">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G121">
-        <v>9</v>
+        <v>7.94</v>
       </c>
       <c r="H121">
-        <v>7.94</v>
-      </c>
-      <c r="I121">
         <v>8</v>
       </c>
     </row>
@@ -4376,24 +3771,19 @@
       <c r="C122">
         <v>5</v>
       </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D122">
+        <v>1</v>
       </c>
       <c r="E122">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F122">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G122">
-        <v>6</v>
+        <v>3.64</v>
       </c>
       <c r="H122">
-        <v>3.64</v>
-      </c>
-      <c r="I122">
         <v>0.5</v>
       </c>
     </row>
@@ -4409,24 +3799,19 @@
       <c r="C123">
         <v>5</v>
       </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D123">
+        <v>1</v>
       </c>
       <c r="E123">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F123">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G123">
-        <v>5</v>
+        <v>3.25</v>
       </c>
       <c r="H123">
-        <v>3.25</v>
-      </c>
-      <c r="I123">
         <v>2</v>
       </c>
     </row>
@@ -4442,24 +3827,19 @@
       <c r="C124">
         <v>5</v>
       </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D124">
+        <v>1</v>
       </c>
       <c r="E124">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F124">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>1.62</v>
       </c>
       <c r="H124">
-        <v>1.62</v>
-      </c>
-      <c r="I124">
         <v>3.5</v>
       </c>
     </row>
@@ -4475,24 +3855,19 @@
       <c r="C125">
         <v>5</v>
       </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D125">
+        <v>1</v>
       </c>
       <c r="E125">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F125">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G125">
-        <v>2</v>
+        <v>2.62</v>
       </c>
       <c r="H125">
-        <v>2.62</v>
-      </c>
-      <c r="I125">
         <v>4</v>
       </c>
     </row>
@@ -4508,24 +3883,19 @@
       <c r="C126">
         <v>5</v>
       </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D126">
+        <v>1</v>
       </c>
       <c r="E126">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F126">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G126">
-        <v>4</v>
+        <v>2.07</v>
       </c>
       <c r="H126">
-        <v>2.07</v>
-      </c>
-      <c r="I126">
         <v>2</v>
       </c>
     </row>
@@ -4541,24 +3911,19 @@
       <c r="C127">
         <v>5</v>
       </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D127">
+        <v>1</v>
       </c>
       <c r="E127">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F127">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G127">
-        <v>3</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="H127">
-        <v>9.050000000000001</v>
-      </c>
-      <c r="I127">
         <v>4.5</v>
       </c>
     </row>
@@ -4574,24 +3939,19 @@
       <c r="C128">
         <v>10</v>
       </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D128">
+        <v>1</v>
       </c>
       <c r="E128">
         <v>1</v>
       </c>
       <c r="F128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G128">
-        <v>2</v>
+        <v>0.54</v>
       </c>
       <c r="H128">
-        <v>0.54</v>
-      </c>
-      <c r="I128">
         <v>2</v>
       </c>
     </row>
@@ -4607,24 +3967,19 @@
       <c r="C129">
         <v>10</v>
       </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D129">
+        <v>1</v>
       </c>
       <c r="E129">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F129">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G129">
-        <v>1</v>
+        <v>5.22</v>
       </c>
       <c r="H129">
-        <v>5.22</v>
-      </c>
-      <c r="I129">
         <v>5</v>
       </c>
     </row>
@@ -4640,24 +3995,19 @@
       <c r="C130">
         <v>10</v>
       </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D130">
+        <v>1</v>
       </c>
       <c r="E130">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F130">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G130">
-        <v>8</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="H130">
-        <v>9.369999999999999</v>
-      </c>
-      <c r="I130">
         <v>5</v>
       </c>
     </row>
@@ -4673,24 +4023,19 @@
       <c r="C131">
         <v>10</v>
       </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D131">
+        <v>1</v>
       </c>
       <c r="E131">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F131">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G131">
-        <v>10</v>
+        <v>7.69</v>
       </c>
       <c r="H131">
-        <v>7.69</v>
-      </c>
-      <c r="I131">
         <v>4</v>
       </c>
     </row>
@@ -4706,24 +4051,19 @@
       <c r="C132">
         <v>10</v>
       </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D132">
+        <v>1</v>
       </c>
       <c r="E132">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F132">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G132">
-        <v>9</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="H132">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="I132">
         <v>8</v>
       </c>
     </row>
@@ -4739,24 +4079,19 @@
       <c r="C133">
         <v>10</v>
       </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D133">
+        <v>1</v>
       </c>
       <c r="E133">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F133">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G133">
-        <v>7</v>
+        <v>5.92</v>
       </c>
       <c r="H133">
-        <v>5.92</v>
-      </c>
-      <c r="I133">
         <v>4.8</v>
       </c>
     </row>
@@ -4772,24 +4107,19 @@
       <c r="C134">
         <v>10</v>
       </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D134">
+        <v>1</v>
       </c>
       <c r="E134">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F134">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G134">
-        <v>6</v>
+        <v>5.95</v>
       </c>
       <c r="H134">
-        <v>5.95</v>
-      </c>
-      <c r="I134">
         <v>6.5</v>
       </c>
     </row>
@@ -4805,24 +4135,19 @@
       <c r="C135">
         <v>10</v>
       </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D135">
+        <v>1</v>
       </c>
       <c r="E135">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F135">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G135">
-        <v>3</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="H135">
-        <v>8.449999999999999</v>
-      </c>
-      <c r="I135">
         <v>5</v>
       </c>
     </row>
@@ -4838,26 +4163,21 @@
       <c r="C136">
         <v>10</v>
       </c>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D136">
+        <v>1</v>
       </c>
       <c r="E136">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F136">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G136">
-        <v>5</v>
+        <v>7.23</v>
       </c>
       <c r="H136">
         <v>7.23</v>
       </c>
-      <c r="I136">
-        <v>7.23</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137">
@@ -4871,24 +4191,19 @@
       <c r="C137">
         <v>10</v>
       </c>
-      <c r="D137" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="D137">
+        <v>1</v>
       </c>
       <c r="E137">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F137">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G137">
-        <v>4</v>
+        <v>2.9</v>
       </c>
       <c r="H137">
-        <v>2.9</v>
-      </c>
-      <c r="I137">
         <v>2</v>
       </c>
     </row>
@@ -4904,24 +4219,19 @@
       <c r="C138">
         <v>5</v>
       </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D138">
+        <v>1</v>
       </c>
       <c r="E138">
         <v>1</v>
       </c>
       <c r="F138">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G138">
-        <v>6</v>
+        <v>0.65</v>
       </c>
       <c r="H138">
-        <v>0.65</v>
-      </c>
-      <c r="I138">
         <v>2</v>
       </c>
     </row>
@@ -4937,24 +4247,19 @@
       <c r="C139">
         <v>5</v>
       </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D139">
+        <v>1</v>
       </c>
       <c r="E139">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F139">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G139">
-        <v>5</v>
+        <v>1.12</v>
       </c>
       <c r="H139">
-        <v>1.12</v>
-      </c>
-      <c r="I139">
         <v>0.52</v>
       </c>
     </row>
@@ -4970,24 +4275,19 @@
       <c r="C140">
         <v>5</v>
       </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D140">
+        <v>1</v>
       </c>
       <c r="E140">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F140">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G140">
-        <v>8</v>
+        <v>0.51</v>
       </c>
       <c r="H140">
-        <v>0.51</v>
-      </c>
-      <c r="I140">
         <v>2</v>
       </c>
     </row>
@@ -5003,24 +4303,19 @@
       <c r="C141">
         <v>5</v>
       </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D141">
+        <v>1</v>
       </c>
       <c r="E141">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F141">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G141">
-        <v>10</v>
+        <v>4.05</v>
       </c>
       <c r="H141">
-        <v>4.05</v>
-      </c>
-      <c r="I141">
         <v>1.13</v>
       </c>
     </row>
@@ -5036,24 +4331,19 @@
       <c r="C142">
         <v>5</v>
       </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D142">
+        <v>1</v>
       </c>
       <c r="E142">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F142">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G142">
-        <v>2</v>
+        <v>0.84</v>
       </c>
       <c r="H142">
-        <v>0.84</v>
-      </c>
-      <c r="I142">
         <v>2.1</v>
       </c>
     </row>
@@ -5069,24 +4359,19 @@
       <c r="C143">
         <v>5</v>
       </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D143">
+        <v>1</v>
       </c>
       <c r="E143">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F143">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G143">
-        <v>1</v>
+        <v>4.32</v>
       </c>
       <c r="H143">
-        <v>4.32</v>
-      </c>
-      <c r="I143">
         <v>2</v>
       </c>
     </row>
@@ -5102,24 +4387,19 @@
       <c r="C144">
         <v>5</v>
       </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D144">
+        <v>1</v>
       </c>
       <c r="E144">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F144">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G144">
-        <v>9</v>
+        <v>2.11</v>
       </c>
       <c r="H144">
-        <v>2.11</v>
-      </c>
-      <c r="I144">
         <v>2</v>
       </c>
     </row>
@@ -5135,24 +4415,19 @@
       <c r="C145">
         <v>5</v>
       </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D145">
+        <v>1</v>
       </c>
       <c r="E145">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F145">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G145">
-        <v>3</v>
+        <v>2.93</v>
       </c>
       <c r="H145">
-        <v>2.93</v>
-      </c>
-      <c r="I145">
         <v>1.78</v>
       </c>
     </row>
@@ -5168,24 +4443,19 @@
       <c r="C146">
         <v>5</v>
       </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D146">
+        <v>1</v>
       </c>
       <c r="E146">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F146">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G146">
-        <v>7</v>
+        <v>4.26</v>
       </c>
       <c r="H146">
-        <v>4.26</v>
-      </c>
-      <c r="I146">
         <v>2.5</v>
       </c>
     </row>
@@ -5201,24 +4471,19 @@
       <c r="C147">
         <v>5</v>
       </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
+      <c r="D147">
+        <v>1</v>
       </c>
       <c r="E147">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F147">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G147">
-        <v>4</v>
+        <v>4.92</v>
       </c>
       <c r="H147">
-        <v>4.92</v>
-      </c>
-      <c r="I147">
         <v>2.9</v>
       </c>
     </row>

</xml_diff>